<commit_message>
Adopted pandas.DataFrame.styler for to_latex
DataFrame.to_latex is deprecated; moving to a styler. What a remarkable PITA.
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0628BCA8-49F1-4382-AE6A-8077E01914F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A84EA7-295E-4A96-A4C3-9702C1A91B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
     <sheet name="EJ44" sheetId="6" r:id="rId2"/>
     <sheet name="EJ45" sheetId="1" r:id="rId3"/>
-    <sheet name="EJ46" sheetId="4" r:id="rId4"/>
-    <sheet name="EJ45FF" sheetId="7" r:id="rId5"/>
-    <sheet name="EJ46FF" sheetId="8" r:id="rId6"/>
+    <sheet name="EJ45 (2)" sheetId="9" r:id="rId4"/>
+    <sheet name="EJ46" sheetId="4" r:id="rId5"/>
+    <sheet name="EJ45FF" sheetId="7" r:id="rId6"/>
+    <sheet name="EJ46FF" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="13">
   <si>
     <t>dx</t>
   </si>
@@ -61,13 +62,31 @@
   <si>
     <t>String 6</t>
   </si>
+  <si>
+    <t>J4501</t>
+  </si>
+  <si>
+    <t>J4502</t>
+  </si>
+  <si>
+    <t>J4503</t>
+  </si>
+  <si>
+    <t>J4504</t>
+  </si>
+  <si>
+    <t>J4505</t>
+  </si>
+  <si>
+    <t>J4506</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -100,10 +119,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,7 +675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66F5002-5E53-46DA-A969-797B9E6035D8}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -668,22 +689,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -853,6 +874,208 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A2DC8E-87F3-4DDB-ACF3-825FAA7EBC5F}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>328.6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>241</v>
+      </c>
+      <c r="D2" s="1">
+        <v>191.6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>144.80000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>109.7</v>
+      </c>
+      <c r="G2" s="2">
+        <v>80.900000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>334.3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>246</v>
+      </c>
+      <c r="D3" s="1">
+        <v>199.1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>148.1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>112</v>
+      </c>
+      <c r="G3" s="2">
+        <v>83.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>340.7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>252</v>
+      </c>
+      <c r="D4" s="1">
+        <v>205.7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>151</v>
+      </c>
+      <c r="F4" s="2">
+        <v>114</v>
+      </c>
+      <c r="G4" s="2">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>346.7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>256</v>
+      </c>
+      <c r="D5" s="1">
+        <v>212.7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>153.4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>116.6</v>
+      </c>
+      <c r="G5" s="2">
+        <v>88.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>352.5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>259.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>216</v>
+      </c>
+      <c r="E6" s="2">
+        <v>156.6</v>
+      </c>
+      <c r="F6" s="2">
+        <v>119</v>
+      </c>
+      <c r="G6" s="2">
+        <v>90.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>359.2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>265</v>
+      </c>
+      <c r="D7" s="1">
+        <v>220.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>158.9</v>
+      </c>
+      <c r="F7" s="2">
+        <v>120.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>93.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>366.7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>270.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>227.3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>160.69999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>122.3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>95.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DCB10-D7CE-45DD-94ED-1A13662D2FAF}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -970,7 +1193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40161EBB-11F4-4250-88CC-7490DDC82810}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1088,11 +1311,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F174DE-CC2E-4D4C-A29D-1F98FEBEDE90}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
EJ45 tables and plots updated
All of the tables and plots for EJ45 strings have been updated. The new fit plot has been added, and the plotting code has been significantly simplified.
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A84EA7-295E-4A96-A4C3-9702C1A91B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB721EDD-0062-44A5-835F-37DD5CD87599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
     <sheet name="EJ44" sheetId="6" r:id="rId2"/>
     <sheet name="EJ45" sheetId="1" r:id="rId3"/>
-    <sheet name="EJ45 (2)" sheetId="9" r:id="rId4"/>
-    <sheet name="EJ46" sheetId="4" r:id="rId5"/>
-    <sheet name="EJ45FF" sheetId="7" r:id="rId6"/>
-    <sheet name="EJ46FF" sheetId="8" r:id="rId7"/>
+    <sheet name="EJ46" sheetId="4" r:id="rId4"/>
+    <sheet name="EJ45FF" sheetId="7" r:id="rId5"/>
+    <sheet name="EJ46FF" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>dx</t>
   </si>
@@ -439,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E08288C-F451-488C-ADF5-051FF7808691}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G8"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66F5002-5E53-46DA-A969-797B9E6035D8}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -874,208 +873,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A2DC8E-87F3-4DDB-ACF3-825FAA7EBC5F}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>328.6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>241</v>
-      </c>
-      <c r="D2" s="1">
-        <v>191.6</v>
-      </c>
-      <c r="E2" s="2">
-        <v>144.80000000000001</v>
-      </c>
-      <c r="F2" s="2">
-        <v>109.7</v>
-      </c>
-      <c r="G2" s="2">
-        <v>80.900000000000006</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>334.3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>246</v>
-      </c>
-      <c r="D3" s="1">
-        <v>199.1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>148.1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>112</v>
-      </c>
-      <c r="G3" s="2">
-        <v>83.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>340.7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>252</v>
-      </c>
-      <c r="D4" s="1">
-        <v>205.7</v>
-      </c>
-      <c r="E4" s="2">
-        <v>151</v>
-      </c>
-      <c r="F4" s="2">
-        <v>114</v>
-      </c>
-      <c r="G4" s="2">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>346.7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>256</v>
-      </c>
-      <c r="D5" s="1">
-        <v>212.7</v>
-      </c>
-      <c r="E5" s="2">
-        <v>153.4</v>
-      </c>
-      <c r="F5" s="2">
-        <v>116.6</v>
-      </c>
-      <c r="G5" s="2">
-        <v>88.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2">
-        <v>352.5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>259.5</v>
-      </c>
-      <c r="D6" s="1">
-        <v>216</v>
-      </c>
-      <c r="E6" s="2">
-        <v>156.6</v>
-      </c>
-      <c r="F6" s="2">
-        <v>119</v>
-      </c>
-      <c r="G6" s="2">
-        <v>90.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>359.2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>265</v>
-      </c>
-      <c r="D7" s="1">
-        <v>220.5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>158.9</v>
-      </c>
-      <c r="F7" s="2">
-        <v>120.5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>93.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2">
-        <v>366.7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>270.5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>227.3</v>
-      </c>
-      <c r="E8" s="2">
-        <v>160.69999999999999</v>
-      </c>
-      <c r="F8" s="2">
-        <v>122.3</v>
-      </c>
-      <c r="G8" s="2">
-        <v>95.9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DCB10-D7CE-45DD-94ED-1A13662D2FAF}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1193,7 +990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40161EBB-11F4-4250-88CC-7490DDC82810}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1311,7 +1108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F174DE-CC2E-4D4C-A29D-1F98FEBEDE90}">
   <dimension ref="A1:G8"/>
   <sheetViews>

</xml_diff>

<commit_message>
All EJ43 tables and plots updated.
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB721EDD-0062-44A5-835F-37DD5CD87599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BB579A-4DED-4781-BF0B-4CF5114FFC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>dx</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>J4506</t>
+  </si>
+  <si>
+    <t>J4301</t>
+  </si>
+  <si>
+    <t>J4302</t>
+  </si>
+  <si>
+    <t>J4303</t>
+  </si>
+  <si>
+    <t>J4304</t>
+  </si>
+  <si>
+    <t>J4305</t>
+  </si>
+  <si>
+    <t>J4306</t>
   </si>
 </sst>
 </file>
@@ -439,7 +457,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,100 +470,184 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="2">
+        <v>298.60000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <v>221.8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>173.8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>133.69999999999999</v>
+      </c>
+      <c r="F2" s="2">
+        <v>98.4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>71.5</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="2">
+        <v>309.2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>229.3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>183.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>136.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100.8</v>
+      </c>
+      <c r="G3" s="2">
+        <v>73.5</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="2">
+        <v>320.39999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>238.7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>192.2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="F4" s="2">
+        <v>102.9</v>
+      </c>
+      <c r="G4" s="2">
+        <v>74.8</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="2">
+        <v>330.3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>248.2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>201.1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>144.80000000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>105</v>
+      </c>
+      <c r="G5" s="2">
+        <v>76.7</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="2">
+        <v>340.5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>257.2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>209.7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>148.69999999999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>107.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>79.400000000000006</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="2">
+        <v>350.5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>265.2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>218.2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>151.9</v>
+      </c>
+      <c r="F7" s="2">
+        <v>109.8</v>
+      </c>
+      <c r="G7" s="2">
+        <v>81.3</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="2">
+        <v>359.2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>271.7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>226.9</v>
+      </c>
+      <c r="E8" s="2">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>112.7</v>
+      </c>
+      <c r="G8" s="2">
+        <v>82.6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added data, fits, graphs for EJ46.
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BB579A-4DED-4781-BF0B-4CF5114FFC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABC5791-9FF3-4B97-822D-31A35B4DB4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>dx</t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>J4306</t>
+  </si>
+  <si>
+    <t>J4601</t>
+  </si>
+  <si>
+    <t>J4602</t>
+  </si>
+  <si>
+    <t>J4603</t>
+  </si>
+  <si>
+    <t>J4604</t>
+  </si>
+  <si>
+    <t>J4605</t>
+  </si>
+  <si>
+    <t>J4606</t>
   </si>
 </sst>
 </file>
@@ -456,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E08288C-F451-488C-ADF5-051FF7808691}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -978,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DCB10-D7CE-45DD-94ED-1A13662D2FAF}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G8"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,100 +1010,184 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="2">
+        <v>297.7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>219.8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>177.4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>132.80000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>98.7</v>
+      </c>
+      <c r="G2" s="2">
+        <v>74.2</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="2">
+        <v>304.39999999999998</v>
+      </c>
+      <c r="C3" s="1">
+        <v>225</v>
+      </c>
+      <c r="D3" s="1">
+        <v>181.7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>135.69999999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100.6</v>
+      </c>
+      <c r="G3" s="2">
+        <v>75.7</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="2">
+        <v>312.2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>230</v>
+      </c>
+      <c r="D4" s="1">
+        <v>187.4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>138</v>
+      </c>
+      <c r="F4" s="2">
+        <v>102.9</v>
+      </c>
+      <c r="G4" s="2">
+        <v>77.599999999999994</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="2">
+        <v>317.89999999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>235</v>
+      </c>
+      <c r="D5" s="1">
+        <v>192.8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>141.1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>105.1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>79.400000000000006</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="2">
+        <v>323.8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>240.6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>196.3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>143.5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>107.2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="2">
+        <v>329.2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>245.9</v>
+      </c>
+      <c r="D7" s="1">
+        <v>200.1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>146.5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>109.4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>82.8</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="2">
+        <v>336.1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>251.6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>204.3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>149.1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>111.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>84.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New data/tables/figures for EJ44 (Extra Hard)
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABC5791-9FF3-4B97-822D-31A35B4DB4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD85443-160F-41BC-BA9B-CBB2F0190848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>dx</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>J4606</t>
+  </si>
+  <si>
+    <t>J4401</t>
+  </si>
+  <si>
+    <t>J4402</t>
+  </si>
+  <si>
+    <t>J4403</t>
+  </si>
+  <si>
+    <t>J4404</t>
+  </si>
+  <si>
+    <t>J4405</t>
+  </si>
+  <si>
+    <t>J4406</t>
   </si>
 </sst>
 </file>
@@ -676,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340D5FFE-12F2-4CBA-BF3F-DC131320B566}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G8"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,100 +708,184 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="2">
+        <v>293.8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>220.1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>177.7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>132.69999999999999</v>
+      </c>
+      <c r="F2" s="2">
+        <v>97.7</v>
+      </c>
+      <c r="G2" s="2">
+        <v>74.5</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="2">
+        <v>299.8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>227.3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>182.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>135.19999999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>99.8</v>
+      </c>
+      <c r="G3" s="2">
+        <v>76.3</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="2">
+        <v>307.5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>235.8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>188.1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="F4" s="2">
+        <v>101.7</v>
+      </c>
+      <c r="G4" s="2">
+        <v>78.099999999999994</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="2">
+        <v>315.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>242.7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>192.8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>142</v>
+      </c>
+      <c r="F5" s="2">
+        <v>104.1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="2">
+        <v>322</v>
+      </c>
+      <c r="C6" s="1">
+        <v>248.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>196.9</v>
+      </c>
+      <c r="E6" s="2">
+        <v>144.80000000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>106.1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>81.7</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="2">
+        <v>328.3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>254.1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>201.2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>147.30000000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>108.2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>83.5</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="2">
+        <v>334.7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>260.3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>206.4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>150.5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>110.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>85.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -996,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DCB10-D7CE-45DD-94ED-1A13662D2FAF}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates to cgic: EJ45FF
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD85443-160F-41BC-BA9B-CBB2F0190848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EB2E8C-0E80-43C0-99CC-6F9E65DF2FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>dx</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>J4406</t>
+  </si>
+  <si>
+    <t>J4501FF</t>
+  </si>
+  <si>
+    <t>J4502FF</t>
+  </si>
+  <si>
+    <t>J4503FF</t>
+  </si>
+  <si>
+    <t>J4504FF</t>
+  </si>
+  <si>
+    <t>J4505FF</t>
+  </si>
+  <si>
+    <t>J4506FF</t>
   </si>
 </sst>
 </file>
@@ -694,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340D5FFE-12F2-4CBA-BF3F-DC131320B566}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1300,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40161EBB-11F4-4250-88CC-7490DDC82810}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G8"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,100 +1332,184 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="2">
+        <v>291.7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>215</v>
+      </c>
+      <c r="D2" s="1">
+        <v>174</v>
+      </c>
+      <c r="E2" s="2">
+        <v>131.9</v>
+      </c>
+      <c r="F2" s="2">
+        <v>98.2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>73.8</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="2">
+        <v>297.5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>220.4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>179.1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>134.80000000000001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100.5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>76</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="2">
+        <v>304.39999999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>226.7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>183.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>138.1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>102.7</v>
+      </c>
+      <c r="G4" s="2">
+        <v>77.599999999999994</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="2">
+        <v>310.5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>232.3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>188.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>141.19999999999999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>105</v>
+      </c>
+      <c r="G5" s="2">
+        <v>79.2</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="2">
+        <v>315.89999999999998</v>
+      </c>
+      <c r="C6" s="1">
+        <v>236.1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>192.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>143.9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>107.8</v>
+      </c>
+      <c r="G6" s="2">
+        <v>80.8</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="2">
+        <v>320.7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>241.8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>195.8</v>
+      </c>
+      <c r="E7" s="2">
+        <v>146.5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>110.2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>81.900000000000006</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="2">
+        <v>327.10000000000002</v>
+      </c>
+      <c r="C8" s="1">
+        <v>246.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>199.9</v>
+      </c>
+      <c r="E8" s="2">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>112.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>83.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepped for EJ46FF measurements.
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EB2E8C-0E80-43C0-99CC-6F9E65DF2FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8916BD6-85F4-4BAC-B08A-1D5A894853C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="4500" yWindow="4500" windowWidth="28800" windowHeight="17685" activeTab="5" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -44,24 +44,6 @@
     <t>dx</t>
   </si>
   <si>
-    <t>String 1</t>
-  </si>
-  <si>
-    <t>String 2</t>
-  </si>
-  <si>
-    <t>String 3</t>
-  </si>
-  <si>
-    <t>String 4</t>
-  </si>
-  <si>
-    <t>String 5</t>
-  </si>
-  <si>
-    <t>String 6</t>
-  </si>
-  <si>
     <t>J4501</t>
   </si>
   <si>
@@ -150,6 +132,24 @@
   </si>
   <si>
     <t>J4506FF</t>
+  </si>
+  <si>
+    <t>J4601FF</t>
+  </si>
+  <si>
+    <t>J4602FF</t>
+  </si>
+  <si>
+    <t>J4603FF</t>
+  </si>
+  <si>
+    <t>J4604FF</t>
+  </si>
+  <si>
+    <t>J4605FF</t>
+  </si>
+  <si>
+    <t>J4606FF</t>
   </si>
 </sst>
 </file>
@@ -514,35 +514,35 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -588,7 +588,7 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -611,7 +611,7 @@
         <v>74.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -634,7 +634,7 @@
         <v>76.7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -657,7 +657,7 @@
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -680,7 +680,7 @@
         <v>81.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -716,35 +716,35 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -767,7 +767,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -790,7 +790,7 @@
         <v>76.3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -813,7 +813,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -836,7 +836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -859,7 +859,7 @@
         <v>81.7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -882,7 +882,7 @@
         <v>83.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -918,35 +918,35 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -969,7 +969,7 @@
         <v>81.900000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -992,7 +992,7 @@
         <v>84.1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>85.7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>87.6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>89.7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>91.6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1120,35 +1120,35 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>77.599999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>82.8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1318,39 +1318,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40161EBB-11F4-4250-88CC-7490DDC82810}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>73.8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>77.599999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>79.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>80.8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>81.900000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1520,39 +1520,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F174DE-CC2E-4D4C-A29D-1F98FEBEDE90}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G8"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1563,7 +1563,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -1574,7 +1574,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1585,7 +1585,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -1618,7 +1618,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
EJ46FF data added and compiled
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8916BD6-85F4-4BAC-B08A-1D5A894853C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390A3C83-E5CC-4795-802F-65485E0868E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="4500" windowWidth="28800" windowHeight="17685" activeTab="5" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -514,12 +514,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -588,7 +588,7 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -611,7 +611,7 @@
         <v>74.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -634,7 +634,7 @@
         <v>76.7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -657,7 +657,7 @@
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -680,7 +680,7 @@
         <v>81.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -716,12 +716,12 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -767,7 +767,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -790,7 +790,7 @@
         <v>76.3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -813,7 +813,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -836,7 +836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -859,7 +859,7 @@
         <v>81.7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -882,7 +882,7 @@
         <v>83.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -918,12 +918,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -969,7 +969,7 @@
         <v>81.900000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -992,7 +992,7 @@
         <v>84.1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>85.7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>87.6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>89.7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>91.6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1120,12 +1120,12 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>77.599999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>82.8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1322,12 +1322,12 @@
       <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>73.8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>77.599999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>79.2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>80.8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>81.900000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1521,15 +1521,15 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1552,82 +1552,166 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>286.39999999999998</v>
+      </c>
+      <c r="C2" s="1">
+        <v>218.3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>170.7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>130.19999999999999</v>
+      </c>
+      <c r="F2" s="2">
+        <v>94.8</v>
+      </c>
+      <c r="G2" s="2">
+        <v>73.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0.5</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>292.2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>222.3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>174.4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>132.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>96.8</v>
+      </c>
+      <c r="G3" s="2">
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>298.2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>227.9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>179.2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>135.5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>99</v>
+      </c>
+      <c r="G4" s="2">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>232.1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>183.9</v>
+      </c>
+      <c r="E5" s="2">
+        <v>137.9</v>
+      </c>
+      <c r="F5" s="2">
+        <v>101.2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>309.7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>236.3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>187.7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>140.80000000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>103.4</v>
+      </c>
+      <c r="G6" s="2">
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2.5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>316</v>
+      </c>
+      <c r="C7" s="1">
+        <v>241.1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>191.4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>143.80000000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>105.4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="2">
+        <v>322.39999999999998</v>
+      </c>
+      <c r="C8" s="1">
+        <v>246.3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>195</v>
+      </c>
+      <c r="E8" s="2">
+        <v>146.69999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>107.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>82.6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes consistent w/JASA format
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390A3C83-E5CC-4795-802F-65485E0868E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CEDA1A-75F6-4B57-BAEB-7EBBA552FF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340D5FFE-12F2-4CBA-BF3F-DC131320B566}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,7 +775,7 @@
         <v>299.8</v>
       </c>
       <c r="C3" s="1">
-        <v>227.3</v>
+        <v>226.1</v>
       </c>
       <c r="D3" s="1">
         <v>182.5</v>
@@ -798,7 +798,7 @@
         <v>307.5</v>
       </c>
       <c r="C4" s="1">
-        <v>235.8</v>
+        <v>233.2</v>
       </c>
       <c r="D4" s="1">
         <v>188.1</v>
@@ -821,7 +821,7 @@
         <v>315.2</v>
       </c>
       <c r="C5" s="1">
-        <v>242.7</v>
+        <v>238.9</v>
       </c>
       <c r="D5" s="1">
         <v>192.8</v>
@@ -844,7 +844,7 @@
         <v>322</v>
       </c>
       <c r="C6" s="1">
-        <v>248.5</v>
+        <v>243.8</v>
       </c>
       <c r="D6" s="1">
         <v>196.9</v>
@@ -867,7 +867,7 @@
         <v>328.3</v>
       </c>
       <c r="C7" s="1">
-        <v>254.1</v>
+        <v>248.5</v>
       </c>
       <c r="D7" s="1">
         <v>201.2</v>
@@ -890,7 +890,7 @@
         <v>334.7</v>
       </c>
       <c r="C8" s="1">
-        <v>260.3</v>
+        <v>253.6</v>
       </c>
       <c r="D8" s="1">
         <v>206.4</v>
@@ -1520,7 +1520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F174DE-CC2E-4D4C-A29D-1F98FEBEDE90}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added error bars to the fit of EJ45 because it was too easy.
</commit_message>
<xml_diff>
--- a/data/guitar_strings_data.xlsx
+++ b/data/guitar_strings_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CEDA1A-75F6-4B57-BAEB-7EBBA552FF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069539B2-B5C2-4D27-B483-E691D6A82462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="EJ46" sheetId="4" r:id="rId4"/>
     <sheet name="EJ45FF" sheetId="7" r:id="rId5"/>
     <sheet name="EJ46FF" sheetId="8" r:id="rId6"/>
+    <sheet name="EJ45eb" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>dx</t>
   </si>
@@ -159,13 +160,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,12 +194,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -252,7 +260,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -358,7 +366,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -500,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -510,9 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E08288C-F451-488C-ADF5-051FF7808691}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -712,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340D5FFE-12F2-4CBA-BF3F-DC131320B566}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1520,9 +1526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F174DE-CC2E-4D4C-A29D-1F98FEBEDE90}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1716,4 +1720,202 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9CAA10-D63A-4D07-815A-338CEB320A6A}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.78</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D2">
+        <v>0.47</v>
+      </c>
+      <c r="E2">
+        <v>0.33</v>
+      </c>
+      <c r="F2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G2">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>0.76</v>
+      </c>
+      <c r="C3">
+        <v>0.63</v>
+      </c>
+      <c r="D3">
+        <v>0.51</v>
+      </c>
+      <c r="E3">
+        <v>0.32</v>
+      </c>
+      <c r="F3">
+        <v>0.27</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.83</v>
+      </c>
+      <c r="C4">
+        <v>0.63</v>
+      </c>
+      <c r="D4">
+        <v>0.49</v>
+      </c>
+      <c r="E4">
+        <v>0.36</v>
+      </c>
+      <c r="F4">
+        <v>0.31</v>
+      </c>
+      <c r="G4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1.5</v>
+      </c>
+      <c r="B5">
+        <v>0.89</v>
+      </c>
+      <c r="C5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E5">
+        <v>0.39</v>
+      </c>
+      <c r="F5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G5">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.92</v>
+      </c>
+      <c r="C6">
+        <v>0.71</v>
+      </c>
+      <c r="D6">
+        <v>0.54</v>
+      </c>
+      <c r="E6">
+        <v>0.36</v>
+      </c>
+      <c r="F6">
+        <v>0.31</v>
+      </c>
+      <c r="G6">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2.5</v>
+      </c>
+      <c r="B7">
+        <v>0.93</v>
+      </c>
+      <c r="C7">
+        <v>0.72</v>
+      </c>
+      <c r="D7">
+        <v>0.51</v>
+      </c>
+      <c r="E7">
+        <v>0.41</v>
+      </c>
+      <c r="F7">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G7">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.93</v>
+      </c>
+      <c r="C8">
+        <v>0.67</v>
+      </c>
+      <c r="D8">
+        <v>0.51</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F8">
+        <v>0.31</v>
+      </c>
+      <c r="G8">
+        <v>0.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>